<commit_message>
testdata updated and excel reader class
</commit_message>
<xml_diff>
--- a/Testdata/testdata.xlsx
+++ b/Testdata/testdata.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef02e7efebdbf4c2/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91861\eclipse-workspace_clone\SeleniumFrameworkFromScratch\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{FE3A8D04-3A95-4E7E-8879-CF134A2F6F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FB06FD7-EEC2-4102-B84B-21462AEDB276}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4BDC56-EBA9-4AEF-8B99-E5E3FB864B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="2540" windowWidth="14400" windowHeight="7270" xr2:uid="{F9E17545-CCC0-4099-B476-3967078589D5}"/>
+    <workbookView xWindow="2220" yWindow="2190" windowWidth="14400" windowHeight="7270" xr2:uid="{F9E17545-CCC0-4099-B476-3967078589D5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Credential" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -418,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F936DB-1F36-4762-ABA4-B52B361D5FB3}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -451,47 +451,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>